<commit_message>
fix lantana content html z-index for rykv
</commit_message>
<xml_diff>
--- a/document/気分記録アプリケーション_lantana_画面一覧.xlsx
+++ b/document/気分記録アプリケーション_lantana_画面一覧.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamat\Git\lantana\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445E3CE-02FA-4CAE-BFFD-BFDD59959E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C9F4A5-0C61-4DA6-B917-FB9E3C0F0141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,23 +17,23 @@
     <sheet name="11" sheetId="1" r:id="rId2"/>
     <sheet name="12" sheetId="2" r:id="rId3"/>
     <sheet name="13" sheetId="3" r:id="rId4"/>
-    <sheet name="21" sheetId="4" r:id="rId5"/>
-    <sheet name="22" sheetId="5" r:id="rId6"/>
-    <sheet name="31" sheetId="6" r:id="rId7"/>
-    <sheet name="32" sheetId="7" r:id="rId8"/>
-    <sheet name="33" sheetId="8" r:id="rId9"/>
-    <sheet name="34" sheetId="9" r:id="rId10"/>
-    <sheet name="35" sheetId="10" r:id="rId11"/>
-    <sheet name="36" sheetId="11" r:id="rId12"/>
-    <sheet name="41" sheetId="12" r:id="rId13"/>
-    <sheet name="42" sheetId="13" r:id="rId14"/>
-    <sheet name="43" sheetId="14" r:id="rId15"/>
-    <sheet name="44" sheetId="15" r:id="rId16"/>
-    <sheet name="51" sheetId="16" r:id="rId17"/>
-    <sheet name="aa" sheetId="17" r:id="rId18"/>
-    <sheet name="ab" sheetId="18" r:id="rId19"/>
-    <sheet name="ac" sheetId="19" r:id="rId20"/>
-    <sheet name="ba" sheetId="20" r:id="rId21"/>
+    <sheet name="14" sheetId="20" r:id="rId5"/>
+    <sheet name="21" sheetId="4" r:id="rId6"/>
+    <sheet name="22" sheetId="5" r:id="rId7"/>
+    <sheet name="31" sheetId="6" r:id="rId8"/>
+    <sheet name="32" sheetId="7" r:id="rId9"/>
+    <sheet name="33" sheetId="8" r:id="rId10"/>
+    <sheet name="34" sheetId="9" r:id="rId11"/>
+    <sheet name="35" sheetId="10" r:id="rId12"/>
+    <sheet name="36" sheetId="11" r:id="rId13"/>
+    <sheet name="41" sheetId="12" r:id="rId14"/>
+    <sheet name="42" sheetId="13" r:id="rId15"/>
+    <sheet name="43" sheetId="14" r:id="rId16"/>
+    <sheet name="44" sheetId="15" r:id="rId17"/>
+    <sheet name="51" sheetId="16" r:id="rId18"/>
+    <sheet name="aa" sheetId="17" r:id="rId19"/>
+    <sheet name="ab" sheetId="18" r:id="rId20"/>
+    <sheet name="ac" sheetId="19" r:id="rId21"/>
     <sheet name="bb" sheetId="21" r:id="rId22"/>
     <sheet name="bc" sheetId="22" r:id="rId23"/>
     <sheet name="bd" sheetId="23" r:id="rId24"/>
@@ -929,7 +929,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3178A03B-5D2A-FF86-DE6E-E8A43E3A86B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{030E5CFA-4DAE-102F-8B02-21BEC66A45EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D827BA01-6710-D272-B11A-72A9E757D757}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3178A03B-5D2A-FF86-DE6E-E8A43E3A86B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1039,7 +1039,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35EC25F-9567-108D-729C-7D764014EB16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D827BA01-6710-D272-B11A-72A9E757D757}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1094,7 +1094,7 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8549A4E4-676E-95E4-ECA9-5967DFC7E64F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35EC25F-9567-108D-729C-7D764014EB16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1126,6 +1126,61 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>124415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8549A4E4-676E-95E4-ECA9-5967DFC7E64F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="5363165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -1155,78 +1210,6 @@
         <a:xfrm>
           <a:off x="4876800" y="942975"/>
           <a:ext cx="342900" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>42</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="テキスト ボックス 4">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F645F3F-20A6-B160-BD02-75E9312B21A0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4048125" y="1266825"/>
-          <a:ext cx="400050" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1265,7 +1248,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>43</a:t>
+            <a:t>42</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -1275,24 +1258,24 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="テキスト ボックス 5">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1D9C9A-A5AA-CC2C-14D8-AC73D637F17A}"/>
+        <xdr:cNvPr id="5" name="テキスト ボックス 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F645F3F-20A6-B160-BD02-75E9312B21A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,14 +1283,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4895850" y="1800225"/>
-          <a:ext cx="400050" cy="276225"/>
+          <a:off x="4048125" y="1266825"/>
+          <a:ext cx="400050" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -1337,6 +1323,81 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>43</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="テキスト ボックス 5">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1D9C9A-A5AA-CC2C-14D8-AC73D637F17A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895850" y="1800225"/>
+          <a:ext cx="400050" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>44</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
@@ -1348,7 +1409,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1403,7 +1464,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1458,7 +1519,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1513,7 +1574,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1568,7 +1629,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1945,7 +2006,212 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>124415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260DDF6A-C77A-8F2A-0BBC-F468D803AD11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="5363165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="テキスト ボックス 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E76CB7A1-9214-6805-FBD8-4DD03BC9089B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7524750" y="990600"/>
+          <a:ext cx="352425" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>12</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="テキスト ボックス 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F46D62B1-410F-0C73-5D53-8A36BDB78FCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7715250" y="190500"/>
+          <a:ext cx="333375" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>22</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2243,212 +2509,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>124415</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260DDF6A-C77A-8F2A-0BBC-F468D803AD11}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7772400" cy="5363165"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="テキスト ボックス 3">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E76CB7A1-9214-6805-FBD8-4DD03BC9089B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7524750" y="990600"/>
-          <a:ext cx="352425" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>12</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="テキスト ボックス 4">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F46D62B1-410F-0C73-5D53-8A36BDB78FCE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7715250" y="190500"/>
-          <a:ext cx="333375" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>22</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2719,61 +2780,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>124415</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842FD568-6143-9B0E-4B12-C30D72482C78}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7772400" cy="5363165"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2920,7 +2926,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>★★★★★</a:t>
+            <a:t>★★★★</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
@@ -2932,7 +2938,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>の気分評価をする。</a:t>
+            <a:t>☆の気分評価をする。</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
             <a:solidFill>
@@ -3418,8 +3424,9 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>左を検索用、右を全件表示用として開く</a:t>
-          </a:r>
+            <a:t>左を検索用、右を全件表示用として開き、検索する。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4153,7 +4160,14 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>気分評価したときの状況を知ることができる。（快晴だった、など）</a:t>
+            <a:t>気分評価したときの状況を知ることができる。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>（快晴だった、など）</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
         </a:p>
@@ -4791,6 +4805,61 @@
         <xdr:cNvPr id="3" name="図 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842FD568-6143-9B0E-4B12-C30D72482C78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="5363165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>124415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D1353E3-C6A5-2358-ED01-6AD83D81FC47}"/>
             </a:ext>
           </a:extLst>
@@ -4976,7 +5045,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5327,7 +5396,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5682,7 +5751,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5703,61 +5772,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F8261DA-36B6-1FDF-54BC-DF6CA105F4F0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7772400" cy="5363165"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>124415</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{030E5CFA-4DAE-102F-8B02-21BEC66A45EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6058,7 +6072,24 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C30ACD8-C3B4-4C32-84EB-B894BE5308F2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6069,7 +6100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7F1869-1C25-4726-9747-71AACC7392FA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6085,7 +6116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39A3D83-6E08-46BE-9930-B41A8B34DEC8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6101,7 +6132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC646802-A3F1-46D4-91F4-E0382648B47B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6117,28 +6148,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB050104-49F7-4310-B9B4-F573E3AE7369}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FE6DEF-3F28-42E6-8E98-C1F899C5E302}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6150,6 +6165,20 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FE6DEF-3F28-42E6-8E98-C1F899C5E302}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A8B76C-0CD5-45B8-9659-B34041E7E098}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6165,7 +6194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06678939-F721-43C6-897E-CC79FEECA7F1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6181,7 +6210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DE8498-D9A1-40FD-AC57-99C57B3EC63A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6197,28 +6226,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E612E6-A590-4ACE-A26A-FE4C75BCA491}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C793DC95-A6B2-4696-B8C5-71C40B90E23B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6233,9 +6246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6247,12 +6258,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07240C41-2720-4383-9ADE-2F93D5703D39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C793DC95-A6B2-4696-B8C5-71C40B90E23B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6263,11 +6272,11 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C862054-D8F3-438C-86B9-4153B624DED1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07240C41-2720-4383-9ADE-2F93D5703D39}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6283,7 +6292,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6298,9 +6307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E875ABA-0FB2-4714-8577-8D173520C9B4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6314,15 +6321,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2591019A-E7F7-4927-9002-CC90CEA23B6A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6331,7 +6337,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6346,9 +6352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8AE176-E9DD-4FB7-B69F-659666326403}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6362,8 +6366,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A685071E-1DF9-4BC1-85C6-1DC277B0E576}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C862054-D8F3-438C-86B9-4153B624DED1}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6374,7 +6392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE72DB2-7FF4-47C4-8FF4-A0165880FB71}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6390,29 +6408,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD47861-CFE9-46CE-BD9F-48A9BA619004}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE38887D-B1D2-474E-9385-54123C320C2D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6423,12 +6423,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957D2B85-9995-4AC5-9E61-58C1860A64D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE38887D-B1D2-474E-9385-54123C320C2D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
@@ -6439,12 +6437,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C30ACD8-C3B4-4C32-84EB-B894BE5308F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957D2B85-9995-4AC5-9E61-58C1860A64D7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>

</xml_diff>